<commit_message>
Added authors gender to assignment file
</commit_message>
<xml_diff>
--- a/13. Metaanalysis/data/metaanalysis_data.xlsx
+++ b/13. Metaanalysis/data/metaanalysis_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whard\OneDrive\Desktop\Reproducible research\RR_classes\RR_classes\may_1014\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whardy\Desktop\RRCourse2023\13. Metaanalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0301A5AA-F45C-4DD7-AB0E-04D66CDCC904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2DE4F6-0204-4F07-BD8A-1DB7D972A2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21732" windowHeight="8532" xr2:uid="{3C303B16-1778-4040-9FE8-FE3707D84BAD}"/>
+    <workbookView xWindow="6735" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{3C303B16-1778-4040-9FE8-FE3707D84BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="47">
   <si>
     <t>Study</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>Female authors</t>
+  </si>
+  <si>
+    <t>Male authors</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -249,9 +255,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -395,7 +401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -545,314 +551,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126B0D72-E236-4C3B-A3F8-91C0ED779F39}">
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
         <v>19.5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2" s="2">
         <v>47</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>47</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>438.72</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="2">
         <v>166.08</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>248.64</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <v>161.28</v>
       </c>
-      <c r="I2" s="3">
+      <c r="K2" s="3">
         <v>377.28</v>
       </c>
-      <c r="J2" s="3">
+      <c r="L2" s="3">
         <v>170.88</v>
       </c>
-      <c r="K2" s="3">
+      <c r="M2" s="3">
         <v>538.55999999999995</v>
       </c>
-      <c r="L2" s="3">
+      <c r="N2" s="3">
         <v>214.08</v>
       </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
         <v>2012</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>3</v>
       </c>
-      <c r="P2" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
+        <v>2</v>
+      </c>
+      <c r="S2" s="2">
         <v>0.25600000000000001</v>
       </c>
-      <c r="R2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s">
-        <v>42</v>
-      </c>
       <c r="T2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X2" t="s">
         <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z2">
+        <v>42</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>19</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E3" s="2">
         <v>22</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>148</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>105</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>54</v>
       </c>
-      <c r="H3" s="2">
+      <c r="J3" s="2">
         <v>53</v>
       </c>
-      <c r="I3" s="3">
+      <c r="K3" s="3">
         <v>126</v>
       </c>
-      <c r="J3" s="3">
+      <c r="L3" s="3">
         <v>67</v>
       </c>
-      <c r="K3" s="3">
+      <c r="M3" s="3">
         <v>244</v>
       </c>
-      <c r="L3" s="3">
+      <c r="N3" s="3">
         <v>54</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>2014</v>
       </c>
-      <c r="O3" s="2">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2">
-        <v>2</v>
-      </c>
       <c r="Q3" s="2">
+        <v>2</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>43</v>
-      </c>
       <c r="T3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U3" t="s">
         <v>43</v>
       </c>
       <c r="V3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" t="s">
         <v>44</v>
       </c>
-      <c r="W3" t="s">
-        <v>42</v>
-      </c>
-      <c r="X3" t="s">
-        <v>42</v>
-      </c>
       <c r="Y3" t="s">
         <v>42</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>65.790000000000006</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E4" s="2">
         <v>18</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>18</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>325.25</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>270.20999999999998</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>135.13</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>201.72</v>
       </c>
-      <c r="I4" s="3">
+      <c r="K4" s="3">
         <v>33.5</v>
       </c>
-      <c r="J4" s="3">
+      <c r="L4" s="3">
         <v>69.55</v>
       </c>
-      <c r="K4" s="3">
+      <c r="M4" s="3">
         <v>247.93</v>
       </c>
-      <c r="L4" s="3">
+      <c r="N4" s="3">
         <v>246.5</v>
       </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
         <v>1992</v>
       </c>
-      <c r="O4" s="2">
-        <v>2</v>
-      </c>
-      <c r="P4" s="2">
-        <v>2</v>
-      </c>
       <c r="Q4" s="2">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
         <v>0.252</v>
       </c>
-      <c r="R4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" t="s">
-        <v>42</v>
-      </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U4" t="s">
         <v>42</v>
@@ -867,75 +891,81 @@
         <v>42</v>
       </c>
       <c r="Y4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z4">
+        <v>42</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
         <v>93.1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="E5" s="2">
         <v>19</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <v>19</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <v>484.21</v>
       </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <v>141.28</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>202.48</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="2">
         <v>168.14</v>
       </c>
-      <c r="I5" s="3">
+      <c r="K5" s="3">
         <v>26.42</v>
       </c>
-      <c r="J5" s="3">
+      <c r="L5" s="3">
         <v>91.95</v>
       </c>
-      <c r="K5" s="3">
+      <c r="M5" s="3">
         <v>265.42</v>
       </c>
-      <c r="L5" s="3">
+      <c r="N5" s="3">
         <v>240.71</v>
       </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
         <v>1995</v>
       </c>
-      <c r="O5" s="2">
-        <v>2</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1</v>
-      </c>
       <c r="Q5" s="2">
+        <v>2</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="2">
         <v>0.252</v>
       </c>
-      <c r="R5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" t="s">
-        <v>43</v>
-      </c>
       <c r="T5" t="s">
         <v>42</v>
       </c>
       <c r="U5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V5" t="s">
         <v>42</v>
@@ -949,228 +979,246 @@
       <c r="Y5" t="s">
         <v>42</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
         <v>87</v>
       </c>
-      <c r="C6" s="2">
+      <c r="E6" s="2">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="2">
         <v>260.10000000000002</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <v>67.7</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <v>98.4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <v>101.3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="K6" s="3">
         <v>7.2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="L6" s="3">
         <v>21.5</v>
       </c>
-      <c r="K6" s="3">
+      <c r="M6" s="3">
         <v>145.19999999999999</v>
       </c>
-      <c r="L6" s="3">
+      <c r="N6" s="3">
         <v>109.6</v>
       </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
         <v>1989</v>
       </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
-      <c r="P6" s="2">
-        <v>2</v>
-      </c>
       <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2">
         <v>0.14099999999999999</v>
       </c>
-      <c r="R6" t="s">
-        <v>42</v>
-      </c>
-      <c r="S6" t="s">
-        <v>42</v>
-      </c>
       <c r="T6" t="s">
         <v>42</v>
       </c>
       <c r="U6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V6" t="s">
         <v>42</v>
       </c>
       <c r="W6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X6" t="s">
         <v>42</v>
       </c>
       <c r="Y6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z6">
+        <v>42</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
         <v>46</v>
       </c>
-      <c r="C7" s="2">
+      <c r="E7" s="2">
         <v>10</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="G7" s="2">
         <v>393.2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="H7" s="2">
         <v>136.19999999999999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <v>271.2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J7" s="2">
         <v>139.69999999999999</v>
       </c>
-      <c r="I7" s="3">
+      <c r="K7" s="3">
         <v>136.6</v>
       </c>
-      <c r="J7" s="3">
+      <c r="L7" s="3">
         <v>92.4</v>
       </c>
-      <c r="K7" s="3">
+      <c r="M7" s="3">
         <v>140.5</v>
       </c>
-      <c r="L7" s="3">
+      <c r="N7" s="3">
         <v>126.8</v>
       </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2">
         <v>1993</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>3</v>
       </c>
-      <c r="P7" s="2">
+      <c r="R7" s="2">
         <v>3</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="S7" s="2">
         <v>0.14099999999999999</v>
       </c>
-      <c r="R7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7" t="s">
-        <v>42</v>
-      </c>
       <c r="T7" t="s">
         <v>42</v>
       </c>
       <c r="U7" t="s">
         <v>42</v>
       </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7">
         <v>0</v>
       </c>
-      <c r="W7" t="s">
-        <v>42</v>
-      </c>
-      <c r="X7" t="s">
-        <v>42</v>
-      </c>
       <c r="Y7" t="s">
         <v>42</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
+      <c r="E8" s="2">
         <v>21</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="2">
         <v>21</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="2">
         <v>46.2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="H8" s="2">
         <v>59.67</v>
       </c>
-      <c r="G8" s="2">
+      <c r="I8" s="2">
         <v>33.54</v>
       </c>
-      <c r="H8" s="2">
+      <c r="J8" s="2">
         <v>47.16</v>
       </c>
-      <c r="I8" s="3">
+      <c r="K8" s="3">
         <v>80.650000000000006</v>
       </c>
-      <c r="J8" s="3">
+      <c r="L8" s="3">
         <v>68.63</v>
       </c>
-      <c r="K8" s="3">
+      <c r="M8" s="3">
         <v>80.09</v>
       </c>
-      <c r="L8" s="3">
+      <c r="N8" s="3">
         <v>79.599999999999994</v>
       </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2">
         <v>2012</v>
       </c>
-      <c r="O8" s="2">
-        <v>2</v>
-      </c>
-      <c r="P8" s="2">
-        <v>2</v>
-      </c>
       <c r="Q8" s="2">
+        <v>2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2">
         <v>0.248</v>
       </c>
-      <c r="R8" t="s">
-        <v>42</v>
-      </c>
-      <c r="S8" t="s">
-        <v>42</v>
-      </c>
       <c r="T8" t="s">
         <v>42</v>
       </c>
@@ -1187,148 +1235,160 @@
         <v>42</v>
       </c>
       <c r="Y8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z8">
+        <v>42</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
         <v>77</v>
       </c>
-      <c r="C9" s="2">
+      <c r="E9" s="2">
         <v>38</v>
       </c>
-      <c r="D9" s="2">
+      <c r="F9" s="2">
         <v>38</v>
       </c>
-      <c r="E9" s="2">
+      <c r="G9" s="2">
         <v>214.7</v>
       </c>
-      <c r="F9" s="2">
+      <c r="H9" s="2">
         <v>132.26</v>
       </c>
-      <c r="G9" s="2">
+      <c r="I9" s="2">
         <v>43.38</v>
       </c>
-      <c r="H9" s="2">
+      <c r="J9" s="2">
         <v>85.79</v>
       </c>
-      <c r="I9" s="3">
+      <c r="K9" s="3">
         <v>26.96</v>
       </c>
-      <c r="J9" s="3">
+      <c r="L9" s="3">
         <v>62.5</v>
       </c>
-      <c r="K9" s="3">
+      <c r="M9" s="3">
         <v>183.28</v>
       </c>
-      <c r="L9" s="3">
+      <c r="N9" s="3">
         <v>117.5</v>
       </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
         <v>2016</v>
       </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" t="s">
-        <v>42</v>
-      </c>
-      <c r="S9" t="s">
-        <v>43</v>
-      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+      <c r="S9" s="2"/>
       <c r="T9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U9" t="s">
         <v>43</v>
       </c>
       <c r="V9" t="s">
+        <v>43</v>
+      </c>
+      <c r="W9" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" t="s">
         <v>44</v>
       </c>
-      <c r="W9" t="s">
-        <v>42</v>
-      </c>
-      <c r="X9" t="s">
-        <v>42</v>
-      </c>
       <c r="Y9" t="s">
         <v>42</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
         <v>81</v>
       </c>
-      <c r="C10" s="2">
+      <c r="E10" s="2">
         <v>12</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="2">
         <v>12</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="2">
         <v>244.8</v>
       </c>
-      <c r="F10" s="2">
+      <c r="H10" s="2">
         <v>118.8</v>
       </c>
-      <c r="G10" s="2">
+      <c r="I10" s="2">
         <v>7.2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="J10" s="2">
         <v>14.4</v>
       </c>
-      <c r="I10" s="3">
+      <c r="K10" s="3">
         <v>21.6</v>
       </c>
-      <c r="J10" s="3">
+      <c r="L10" s="3">
         <v>36</v>
       </c>
-      <c r="K10" s="3">
+      <c r="M10" s="3">
         <v>115.2</v>
       </c>
-      <c r="L10" s="3">
+      <c r="N10" s="3">
         <v>169.2</v>
       </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2">
         <v>2005</v>
       </c>
-      <c r="O10" s="2">
+      <c r="Q10" s="2">
         <v>3</v>
       </c>
-      <c r="P10" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
+        <v>2</v>
+      </c>
+      <c r="S10" s="2">
         <v>0.22800000000000001</v>
       </c>
-      <c r="R10" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" t="s">
-        <v>42</v>
-      </c>
       <c r="T10" t="s">
         <v>42</v>
       </c>
@@ -1345,70 +1405,76 @@
         <v>42</v>
       </c>
       <c r="Y10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z10">
+        <v>42</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
         <v>81</v>
       </c>
-      <c r="C11" s="2">
+      <c r="E11" s="2">
         <v>25</v>
       </c>
-      <c r="D11" s="2">
+      <c r="F11" s="2">
         <v>25</v>
       </c>
-      <c r="E11" s="2">
+      <c r="G11" s="2">
         <v>144</v>
       </c>
-      <c r="F11" s="2">
+      <c r="H11" s="2">
         <v>144</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I11" s="2">
         <v>43.2</v>
       </c>
-      <c r="H11" s="2">
+      <c r="J11" s="2">
         <v>104.4</v>
       </c>
-      <c r="I11" s="3">
+      <c r="K11" s="3">
         <v>43.2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="L11" s="3">
         <v>93.6</v>
       </c>
-      <c r="K11" s="3">
+      <c r="M11" s="3">
         <v>147.6</v>
       </c>
-      <c r="L11" s="3">
+      <c r="N11" s="3">
         <v>169.2</v>
       </c>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2">
         <v>2005</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <v>3</v>
       </c>
-      <c r="P11" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
+        <v>2</v>
+      </c>
+      <c r="S11" s="2">
         <v>0.22800000000000001</v>
       </c>
-      <c r="R11" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" t="s">
-        <v>42</v>
-      </c>
       <c r="T11" t="s">
         <v>42</v>
       </c>
@@ -1425,70 +1491,76 @@
         <v>42</v>
       </c>
       <c r="Y11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z11">
+        <v>42</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
         <v>81</v>
       </c>
-      <c r="C12" s="2">
+      <c r="E12" s="2">
         <v>24</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>24</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2">
         <v>252</v>
       </c>
-      <c r="F12" s="2">
+      <c r="H12" s="2">
         <v>100.8</v>
       </c>
-      <c r="G12" s="2">
+      <c r="I12" s="2">
         <v>46.8</v>
       </c>
-      <c r="H12" s="2">
+      <c r="J12" s="2">
         <v>93.6</v>
       </c>
-      <c r="I12" s="3">
+      <c r="K12" s="3">
         <v>21.6</v>
       </c>
-      <c r="J12" s="3">
+      <c r="L12" s="3">
         <v>68.400000000000006</v>
       </c>
-      <c r="K12" s="3">
+      <c r="M12" s="3">
         <v>219.6</v>
       </c>
-      <c r="L12" s="3">
+      <c r="N12" s="3">
         <v>136.80000000000001</v>
       </c>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12" s="2">
         <v>2005</v>
       </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2">
-        <v>2</v>
-      </c>
       <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2">
+        <v>2</v>
+      </c>
+      <c r="S12" s="2">
         <v>0.22800000000000001</v>
       </c>
-      <c r="R12" t="s">
-        <v>42</v>
-      </c>
-      <c r="S12" t="s">
-        <v>42</v>
-      </c>
       <c r="T12" t="s">
         <v>42</v>
       </c>
@@ -1505,70 +1577,76 @@
         <v>42</v>
       </c>
       <c r="Y12" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z12">
+        <v>42</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="2">
+      <c r="E13" s="2">
         <v>26</v>
       </c>
-      <c r="D13" s="2">
+      <c r="F13" s="2">
         <v>26</v>
       </c>
-      <c r="E13" s="2">
+      <c r="G13" s="2">
         <v>357.04</v>
       </c>
-      <c r="F13" s="2">
+      <c r="H13" s="2">
         <v>209.02</v>
       </c>
-      <c r="G13" s="2">
+      <c r="I13" s="2">
         <v>131.47999999999999</v>
       </c>
-      <c r="H13" s="2">
+      <c r="J13" s="2">
         <v>107.9</v>
       </c>
-      <c r="I13" s="3">
+      <c r="K13" s="3">
         <v>92.08</v>
       </c>
-      <c r="J13" s="3">
+      <c r="L13" s="3">
         <v>102.25</v>
       </c>
-      <c r="K13" s="3">
+      <c r="M13" s="3">
         <v>166.92</v>
       </c>
-      <c r="L13" s="3">
+      <c r="N13" s="3">
         <v>159.62</v>
       </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
         <v>1980</v>
       </c>
-      <c r="O13" s="2">
-        <v>2</v>
-      </c>
-      <c r="P13" s="2">
-        <v>2</v>
-      </c>
       <c r="Q13" s="2">
+        <v>2</v>
+      </c>
+      <c r="R13" s="2">
+        <v>2</v>
+      </c>
+      <c r="S13" s="2">
         <v>0.28799999999999998</v>
       </c>
-      <c r="R13" t="s">
-        <v>42</v>
-      </c>
-      <c r="S13" t="s">
-        <v>42</v>
-      </c>
       <c r="T13" t="s">
         <v>42</v>
       </c>
@@ -1579,7 +1657,7 @@
         <v>42</v>
       </c>
       <c r="W13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X13" t="s">
         <v>42</v>
@@ -1587,79 +1665,85 @@
       <c r="Y13" t="s">
         <v>43</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="E14" s="2">
         <v>19</v>
       </c>
-      <c r="D14" s="2">
+      <c r="F14" s="2">
         <v>19</v>
       </c>
-      <c r="E14" s="2">
+      <c r="G14" s="2">
         <v>182.29</v>
       </c>
-      <c r="F14" s="2">
+      <c r="H14" s="2">
         <v>103.93</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="2">
         <v>114.48</v>
       </c>
-      <c r="H14" s="2">
+      <c r="J14" s="2">
         <v>75.02</v>
       </c>
-      <c r="I14" s="3">
+      <c r="K14" s="3">
         <v>220.82</v>
       </c>
-      <c r="J14" s="3">
+      <c r="L14" s="3">
         <v>103.27</v>
       </c>
-      <c r="K14" s="3">
+      <c r="M14" s="3">
         <v>275.08</v>
       </c>
-      <c r="L14" s="3">
+      <c r="N14" s="3">
         <v>98.2</v>
       </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
         <v>1999</v>
       </c>
-      <c r="O14" s="2">
+      <c r="Q14" s="2">
         <v>3</v>
       </c>
-      <c r="P14" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="R14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S14" t="s">
-        <v>42</v>
-      </c>
       <c r="T14" t="s">
         <v>42</v>
       </c>
       <c r="U14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V14" t="s">
         <v>42</v>
       </c>
       <c r="W14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X14" t="s">
         <v>42</v>
@@ -1667,79 +1751,85 @@
       <c r="Y14" t="s">
         <v>42</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB14">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
         <v>36</v>
       </c>
-      <c r="C15" s="2">
+      <c r="E15" s="2">
         <v>13</v>
       </c>
-      <c r="D15" s="2">
+      <c r="F15" s="2">
         <v>13</v>
       </c>
-      <c r="E15" s="2">
+      <c r="G15" s="2">
         <v>279.88</v>
       </c>
-      <c r="F15" s="2">
+      <c r="H15" s="2">
         <v>67.09</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="2">
         <v>139.75</v>
       </c>
-      <c r="H15" s="2">
+      <c r="J15" s="2">
         <v>77.45</v>
       </c>
-      <c r="I15" s="3">
+      <c r="K15" s="3">
         <v>73.19</v>
       </c>
-      <c r="J15" s="3">
+      <c r="L15" s="3">
         <v>56.9</v>
       </c>
-      <c r="K15" s="3">
+      <c r="M15" s="3">
         <v>215.83</v>
       </c>
-      <c r="L15" s="3">
+      <c r="N15" s="3">
         <v>156.91999999999999</v>
       </c>
-      <c r="M15" s="2">
-        <v>1</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
+        <v>1</v>
+      </c>
+      <c r="P15" s="2">
         <v>1999</v>
       </c>
-      <c r="O15" s="2">
+      <c r="Q15" s="2">
         <v>3</v>
       </c>
-      <c r="P15" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
+        <v>2</v>
+      </c>
+      <c r="S15" s="2">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="R15" t="s">
-        <v>42</v>
-      </c>
-      <c r="S15" t="s">
-        <v>42</v>
-      </c>
       <c r="T15" t="s">
         <v>42</v>
       </c>
       <c r="U15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V15" t="s">
         <v>42</v>
       </c>
       <c r="W15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X15" t="s">
         <v>42</v>
@@ -1747,79 +1837,85 @@
       <c r="Y15" t="s">
         <v>42</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB15">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
         <v>60</v>
       </c>
-      <c r="C16" s="2">
+      <c r="E16" s="2">
         <v>14</v>
       </c>
-      <c r="D16" s="2">
+      <c r="F16" s="2">
         <v>14</v>
       </c>
-      <c r="E16" s="2">
+      <c r="G16" s="2">
         <v>244.07</v>
       </c>
-      <c r="F16" s="2">
+      <c r="H16" s="2">
         <v>123.3</v>
       </c>
-      <c r="G16" s="2">
+      <c r="I16" s="2">
         <v>150.41999999999999</v>
       </c>
-      <c r="H16" s="2">
+      <c r="J16" s="2">
         <v>104.55</v>
       </c>
-      <c r="I16" s="3">
+      <c r="K16" s="3">
         <v>23.75</v>
       </c>
-      <c r="J16" s="3">
+      <c r="L16" s="3">
         <v>44.08</v>
       </c>
-      <c r="K16" s="3">
+      <c r="M16" s="3">
         <v>139.1</v>
       </c>
-      <c r="L16" s="3">
+      <c r="N16" s="3">
         <v>110.38</v>
       </c>
-      <c r="M16" s="2">
-        <v>1</v>
-      </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2">
         <v>1999</v>
       </c>
-      <c r="O16" s="2">
+      <c r="Q16" s="2">
         <v>3</v>
       </c>
-      <c r="P16" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
+        <v>2</v>
+      </c>
+      <c r="S16" s="2">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="R16" t="s">
-        <v>42</v>
-      </c>
-      <c r="S16" t="s">
-        <v>42</v>
-      </c>
       <c r="T16" t="s">
         <v>42</v>
       </c>
       <c r="U16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V16" t="s">
         <v>42</v>
       </c>
       <c r="W16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X16" t="s">
         <v>42</v>
@@ -1827,76 +1923,82 @@
       <c r="Y16" t="s">
         <v>42</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
+      <c r="E17" s="2">
         <v>20</v>
       </c>
-      <c r="D17" s="2">
+      <c r="F17" s="2">
         <v>20</v>
       </c>
-      <c r="E17" s="2">
+      <c r="G17" s="2">
         <v>31.65</v>
       </c>
-      <c r="F17" s="2">
+      <c r="H17" s="2">
         <v>29.15</v>
       </c>
-      <c r="G17" s="2">
+      <c r="I17" s="2">
         <v>5.75</v>
       </c>
-      <c r="H17" s="2">
+      <c r="J17" s="2">
         <v>11.55</v>
       </c>
-      <c r="I17" s="3">
+      <c r="K17" s="3">
         <v>7.35</v>
       </c>
-      <c r="J17" s="3">
+      <c r="L17" s="3">
         <v>13.45</v>
       </c>
-      <c r="K17" s="3">
+      <c r="M17" s="3">
         <v>42.05</v>
       </c>
-      <c r="L17" s="3">
+      <c r="N17" s="3">
         <v>38.35</v>
       </c>
-      <c r="M17" s="2">
+      <c r="O17" s="2">
         <v>0</v>
       </c>
-      <c r="N17" s="2">
+      <c r="P17" s="2">
         <v>2014</v>
       </c>
-      <c r="O17" s="2">
-        <v>2</v>
-      </c>
-      <c r="P17" s="2">
+      <c r="Q17" s="2">
+        <v>2</v>
+      </c>
+      <c r="R17" s="2">
         <v>3</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="S17" s="2">
         <v>0.193</v>
       </c>
-      <c r="R17" t="s">
-        <v>42</v>
-      </c>
-      <c r="S17" t="s">
-        <v>42</v>
-      </c>
       <c r="T17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U17" t="s">
         <v>42</v>
       </c>
       <c r="V17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W17" t="s">
         <v>42</v>
@@ -1907,76 +2009,82 @@
       <c r="Y17" t="s">
         <v>42</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
         <v>21.5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="E18" s="2">
         <v>18</v>
       </c>
-      <c r="D18" s="2">
+      <c r="F18" s="2">
         <v>18</v>
       </c>
-      <c r="E18" s="2">
+      <c r="G18" s="2">
         <v>46.95</v>
       </c>
-      <c r="F18" s="2">
+      <c r="H18" s="2">
         <v>29.7</v>
       </c>
-      <c r="G18" s="2">
+      <c r="I18" s="2">
         <v>12.3</v>
       </c>
-      <c r="H18" s="2">
+      <c r="J18" s="2">
         <v>17.649999999999999</v>
       </c>
-      <c r="I18" s="3">
+      <c r="K18" s="3">
         <v>6.1</v>
       </c>
-      <c r="J18" s="3">
+      <c r="L18" s="3">
         <v>7.4</v>
       </c>
-      <c r="K18" s="3">
+      <c r="M18" s="3">
         <v>57.35</v>
       </c>
-      <c r="L18" s="3">
+      <c r="N18" s="3">
         <v>28.95</v>
       </c>
-      <c r="M18" s="2">
+      <c r="O18" s="2">
         <v>0</v>
       </c>
-      <c r="N18" s="2">
+      <c r="P18" s="2">
         <v>2014</v>
       </c>
-      <c r="O18" s="2">
-        <v>2</v>
-      </c>
-      <c r="P18" s="2">
+      <c r="Q18" s="2">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2">
         <v>3</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="S18" s="2">
         <v>0.193</v>
       </c>
-      <c r="R18" t="s">
-        <v>42</v>
-      </c>
-      <c r="S18" t="s">
-        <v>42</v>
-      </c>
       <c r="T18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U18" t="s">
         <v>42</v>
       </c>
       <c r="V18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W18" t="s">
         <v>42</v>
@@ -1987,76 +2095,82 @@
       <c r="Y18" t="s">
         <v>42</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB18">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
         <v>28</v>
       </c>
-      <c r="C19" s="2">
+      <c r="E19" s="2">
         <v>16</v>
       </c>
-      <c r="D19" s="2">
+      <c r="F19" s="2">
         <v>16</v>
       </c>
-      <c r="E19" s="2">
+      <c r="G19" s="2">
         <v>75</v>
       </c>
-      <c r="F19" s="2">
+      <c r="H19" s="2">
         <v>28.6</v>
       </c>
-      <c r="G19" s="2">
+      <c r="I19" s="2">
         <v>13.6</v>
       </c>
-      <c r="H19" s="2">
+      <c r="J19" s="2">
         <v>17.600000000000001</v>
       </c>
-      <c r="I19" s="3">
+      <c r="K19" s="3">
         <v>14</v>
       </c>
-      <c r="J19" s="3">
+      <c r="L19" s="3">
         <v>17.649999999999999</v>
       </c>
-      <c r="K19" s="3">
+      <c r="M19" s="3">
         <v>58.9</v>
       </c>
-      <c r="L19" s="3">
+      <c r="N19" s="3">
         <v>31.85</v>
       </c>
-      <c r="M19" s="2">
+      <c r="O19" s="2">
         <v>0</v>
       </c>
-      <c r="N19" s="2">
+      <c r="P19" s="2">
         <v>2014</v>
       </c>
-      <c r="O19" s="2">
-        <v>2</v>
-      </c>
-      <c r="P19" s="2">
+      <c r="Q19" s="2">
+        <v>2</v>
+      </c>
+      <c r="R19" s="2">
         <v>3</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="S19" s="2">
         <v>0.193</v>
       </c>
-      <c r="R19" t="s">
-        <v>42</v>
-      </c>
-      <c r="S19" t="s">
-        <v>42</v>
-      </c>
       <c r="T19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U19" t="s">
         <v>42</v>
       </c>
       <c r="V19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W19" t="s">
         <v>42</v>
@@ -2067,319 +2181,343 @@
       <c r="Y19" t="s">
         <v>42</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
         <v>13</v>
       </c>
-      <c r="C20" s="2">
+      <c r="E20" s="2">
         <v>63</v>
       </c>
-      <c r="D20" s="2">
+      <c r="F20" s="2">
         <v>63</v>
       </c>
-      <c r="E20" s="2">
+      <c r="G20" s="2">
         <v>169.98</v>
       </c>
-      <c r="F20" s="2">
+      <c r="H20" s="2">
         <v>118.23</v>
       </c>
-      <c r="G20" s="2">
+      <c r="I20" s="2">
         <v>112.47</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="2">
         <v>94.54</v>
       </c>
-      <c r="I20" s="3">
+      <c r="K20" s="3">
         <v>151.97</v>
       </c>
-      <c r="J20" s="3">
+      <c r="L20" s="3">
         <v>117.28</v>
       </c>
-      <c r="K20" s="3">
+      <c r="M20" s="3">
         <v>189.82</v>
       </c>
-      <c r="L20" s="3">
+      <c r="N20" s="3">
         <v>112.96</v>
       </c>
-      <c r="M20" s="2">
-        <v>1</v>
-      </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
         <v>2009</v>
       </c>
-      <c r="O20" s="2">
-        <v>2</v>
-      </c>
-      <c r="P20" s="2">
-        <v>2</v>
-      </c>
       <c r="Q20" s="2">
+        <v>2</v>
+      </c>
+      <c r="R20" s="2">
+        <v>2</v>
+      </c>
+      <c r="S20" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="R20" t="s">
-        <v>42</v>
-      </c>
-      <c r="S20" t="s">
-        <v>42</v>
-      </c>
       <c r="T20" t="s">
         <v>42</v>
       </c>
       <c r="U20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V20" t="s">
+        <v>42</v>
+      </c>
+      <c r="W20" t="s">
+        <v>43</v>
+      </c>
+      <c r="X20" t="s">
         <v>44</v>
       </c>
-      <c r="W20" t="s">
-        <v>42</v>
-      </c>
-      <c r="X20" t="s">
-        <v>42</v>
-      </c>
       <c r="Y20" t="s">
         <v>42</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
         <v>65.83</v>
       </c>
-      <c r="C21" s="2">
+      <c r="E21" s="2">
         <v>26</v>
       </c>
-      <c r="D21" s="2">
+      <c r="F21" s="2">
         <v>26</v>
       </c>
-      <c r="E21" s="2">
+      <c r="G21" s="2">
         <v>158.33000000000001</v>
       </c>
-      <c r="F21" s="2">
+      <c r="H21" s="2">
         <v>80.790000000000006</v>
       </c>
-      <c r="G21" s="2">
+      <c r="I21" s="2">
         <v>80.45</v>
       </c>
-      <c r="H21" s="2">
+      <c r="J21" s="2">
         <v>66.38</v>
       </c>
-      <c r="I21" s="3">
+      <c r="K21" s="3">
         <v>63.43</v>
       </c>
-      <c r="J21" s="3">
+      <c r="L21" s="3">
         <v>72.290000000000006</v>
       </c>
-      <c r="K21" s="3">
+      <c r="M21" s="3">
         <v>148.30000000000001</v>
       </c>
-      <c r="L21" s="3">
+      <c r="N21" s="3">
         <v>77.38</v>
       </c>
-      <c r="M21" s="2">
+      <c r="O21" s="2">
         <v>0</v>
       </c>
-      <c r="N21" s="2">
+      <c r="P21" s="2">
         <v>2008</v>
       </c>
-      <c r="O21" s="2">
-        <v>2</v>
-      </c>
-      <c r="P21" s="2">
+      <c r="Q21" s="2">
+        <v>2</v>
+      </c>
+      <c r="R21" s="2">
         <v>3</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="S21" s="2">
         <v>0.14299999999999999</v>
       </c>
-      <c r="R21" t="s">
-        <v>42</v>
-      </c>
-      <c r="S21" t="s">
-        <v>42</v>
-      </c>
       <c r="T21" t="s">
         <v>42</v>
       </c>
       <c r="U21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V21" t="s">
         <v>42</v>
       </c>
       <c r="W21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X21" t="s">
         <v>42</v>
       </c>
       <c r="Y21" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z21">
+        <v>42</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
         <v>65.83</v>
       </c>
-      <c r="C22" s="2">
+      <c r="E22" s="2">
         <v>31</v>
       </c>
-      <c r="D22" s="2">
+      <c r="F22" s="2">
         <v>31</v>
       </c>
-      <c r="E22" s="2">
+      <c r="G22" s="2">
         <v>130.88999999999999</v>
       </c>
-      <c r="F22" s="2">
+      <c r="H22" s="2">
         <v>89.36</v>
       </c>
-      <c r="G22" s="2">
+      <c r="I22" s="2">
         <v>82.01</v>
       </c>
-      <c r="H22" s="2">
+      <c r="J22" s="2">
         <v>75.83</v>
       </c>
-      <c r="I22" s="3">
+      <c r="K22" s="3">
         <v>61.52</v>
       </c>
-      <c r="J22" s="3">
+      <c r="L22" s="3">
         <v>74.03</v>
       </c>
-      <c r="K22" s="3">
+      <c r="M22" s="3">
         <v>125.03</v>
       </c>
-      <c r="L22" s="3">
+      <c r="N22" s="3">
         <v>79.319999999999993</v>
       </c>
-      <c r="M22" s="2">
+      <c r="O22" s="2">
         <v>0</v>
       </c>
-      <c r="N22" s="2">
+      <c r="P22" s="2">
         <v>2008</v>
       </c>
-      <c r="O22" s="2">
-        <v>1</v>
-      </c>
-      <c r="P22" s="2">
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2">
         <v>3</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="S22" s="2">
         <v>0.14299999999999999</v>
       </c>
-      <c r="R22" t="s">
-        <v>42</v>
-      </c>
-      <c r="S22" t="s">
-        <v>42</v>
-      </c>
       <c r="T22" t="s">
         <v>42</v>
       </c>
       <c r="U22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V22" t="s">
         <v>42</v>
       </c>
       <c r="W22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X22" t="s">
         <v>42</v>
       </c>
       <c r="Y22" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z22">
+        <v>42</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB22">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
         <v>18</v>
       </c>
-      <c r="C23" s="2">
+      <c r="E23" s="2">
         <v>36</v>
       </c>
-      <c r="D23" s="2">
+      <c r="F23" s="2">
         <v>36</v>
       </c>
-      <c r="E23" s="2">
+      <c r="G23" s="2">
         <v>72</v>
       </c>
-      <c r="F23" s="2">
+      <c r="H23" s="2">
         <v>90</v>
       </c>
-      <c r="G23" s="2">
+      <c r="I23" s="2">
         <v>30</v>
       </c>
-      <c r="H23" s="2">
+      <c r="J23" s="2">
         <v>36</v>
       </c>
-      <c r="I23" s="3">
+      <c r="K23" s="3">
         <v>78</v>
       </c>
-      <c r="J23" s="3">
+      <c r="L23" s="3">
         <v>120</v>
       </c>
-      <c r="K23" s="3">
+      <c r="M23" s="3">
         <v>90</v>
       </c>
-      <c r="L23" s="3">
+      <c r="N23" s="3">
         <v>108</v>
       </c>
-      <c r="M23" s="2">
-        <v>1</v>
-      </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
         <v>2009</v>
       </c>
-      <c r="O23" s="2">
-        <v>2</v>
-      </c>
-      <c r="P23" s="2">
-        <v>1</v>
-      </c>
       <c r="Q23" s="2">
+        <v>2</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
         <v>0.28799999999999998</v>
       </c>
-      <c r="R23" t="s">
-        <v>42</v>
-      </c>
-      <c r="S23" t="s">
-        <v>42</v>
-      </c>
       <c r="T23" t="s">
         <v>42</v>
       </c>
       <c r="U23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V23" t="s">
         <v>42</v>
       </c>
       <c r="W23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X23" t="s">
         <v>42</v>
@@ -2387,79 +2525,85 @@
       <c r="Y23" t="s">
         <v>42</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="2">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
         <v>22</v>
       </c>
-      <c r="C24" s="2">
+      <c r="E24" s="2">
         <v>36</v>
       </c>
-      <c r="D24" s="2">
+      <c r="F24" s="2">
         <v>36</v>
       </c>
-      <c r="E24" s="2">
+      <c r="G24" s="2">
         <v>78</v>
       </c>
-      <c r="F24" s="2">
+      <c r="H24" s="2">
         <v>114</v>
       </c>
-      <c r="G24" s="2">
+      <c r="I24" s="2">
         <v>30</v>
       </c>
-      <c r="H24" s="2">
-        <v>42</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="J24" s="2">
+        <v>42</v>
+      </c>
+      <c r="K24" s="3">
         <v>54</v>
       </c>
-      <c r="J24" s="3">
+      <c r="L24" s="3">
         <v>60</v>
       </c>
-      <c r="K24" s="3">
+      <c r="M24" s="3">
         <v>150</v>
       </c>
-      <c r="L24" s="3">
+      <c r="N24" s="3">
         <v>162</v>
       </c>
-      <c r="M24" s="2">
-        <v>1</v>
-      </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2">
         <v>2009</v>
       </c>
-      <c r="O24" s="2">
-        <v>2</v>
-      </c>
-      <c r="P24" s="2">
-        <v>1</v>
-      </c>
       <c r="Q24" s="2">
+        <v>2</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2">
         <v>0.28799999999999998</v>
       </c>
-      <c r="R24" t="s">
-        <v>42</v>
-      </c>
-      <c r="S24" t="s">
-        <v>42</v>
-      </c>
       <c r="T24" t="s">
         <v>42</v>
       </c>
       <c r="U24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V24" t="s">
         <v>42</v>
       </c>
       <c r="W24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X24" t="s">
         <v>42</v>
@@ -2467,79 +2611,85 @@
       <c r="Y24" t="s">
         <v>42</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB24">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
         <v>18</v>
       </c>
-      <c r="C25" s="2">
+      <c r="E25" s="2">
         <v>36</v>
       </c>
-      <c r="D25" s="2">
+      <c r="F25" s="2">
         <v>36</v>
       </c>
-      <c r="E25" s="2">
+      <c r="G25" s="2">
         <v>54</v>
       </c>
-      <c r="F25" s="2">
+      <c r="H25" s="2">
         <v>84</v>
       </c>
-      <c r="G25" s="2">
-        <v>42</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
+        <v>42</v>
+      </c>
+      <c r="J25" s="2">
         <v>54</v>
       </c>
-      <c r="I25" s="3">
+      <c r="K25" s="3">
         <v>96</v>
       </c>
-      <c r="J25" s="3">
+      <c r="L25" s="3">
         <v>102</v>
       </c>
-      <c r="K25" s="3">
+      <c r="M25" s="3">
         <v>108</v>
       </c>
-      <c r="L25" s="3">
+      <c r="N25" s="3">
         <v>116</v>
       </c>
-      <c r="M25" s="2">
-        <v>1</v>
-      </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2">
         <v>2009</v>
       </c>
-      <c r="O25" s="2">
+      <c r="Q25" s="2">
         <v>3</v>
       </c>
-      <c r="P25" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="2">
+      <c r="R25" s="2">
+        <v>1</v>
+      </c>
+      <c r="S25" s="2">
         <v>0.28799999999999998</v>
       </c>
-      <c r="R25" t="s">
-        <v>42</v>
-      </c>
-      <c r="S25" t="s">
-        <v>42</v>
-      </c>
       <c r="T25" t="s">
         <v>42</v>
       </c>
       <c r="U25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V25" t="s">
         <v>42</v>
       </c>
       <c r="W25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X25" t="s">
         <v>42</v>
@@ -2547,79 +2697,85 @@
       <c r="Y25" t="s">
         <v>42</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="2">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
         <v>22</v>
       </c>
-      <c r="C26" s="2">
+      <c r="E26" s="2">
         <v>36</v>
       </c>
-      <c r="D26" s="2">
+      <c r="F26" s="2">
         <v>36</v>
       </c>
-      <c r="E26" s="2">
+      <c r="G26" s="2">
         <v>66</v>
       </c>
-      <c r="F26" s="2">
+      <c r="H26" s="2">
         <v>66</v>
       </c>
-      <c r="G26" s="2">
+      <c r="I26" s="2">
         <v>36</v>
       </c>
-      <c r="H26" s="2">
+      <c r="J26" s="2">
         <v>84</v>
       </c>
-      <c r="I26" s="3">
+      <c r="K26" s="3">
         <v>78</v>
       </c>
-      <c r="J26" s="3">
+      <c r="L26" s="3">
         <v>84</v>
       </c>
-      <c r="K26" s="3">
+      <c r="M26" s="3">
         <v>120</v>
       </c>
-      <c r="L26" s="3">
+      <c r="N26" s="3">
         <v>136</v>
       </c>
-      <c r="M26" s="2">
-        <v>1</v>
-      </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2">
         <v>2009</v>
       </c>
-      <c r="O26" s="2">
+      <c r="Q26" s="2">
         <v>3</v>
       </c>
-      <c r="P26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="2">
+      <c r="R26" s="2">
+        <v>1</v>
+      </c>
+      <c r="S26" s="2">
         <v>0.28799999999999998</v>
       </c>
-      <c r="R26" t="s">
-        <v>42</v>
-      </c>
-      <c r="S26" t="s">
-        <v>42</v>
-      </c>
       <c r="T26" t="s">
         <v>42</v>
       </c>
       <c r="U26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V26" t="s">
         <v>42</v>
       </c>
       <c r="W26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X26" t="s">
         <v>42</v>
@@ -2627,167 +2783,185 @@
       <c r="Y26" t="s">
         <v>42</v>
       </c>
-      <c r="Z26">
+      <c r="Z26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB26">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="E27" s="2">
         <v>93</v>
       </c>
-      <c r="D27" s="2">
+      <c r="F27" s="2">
         <v>99</v>
       </c>
-      <c r="E27" s="2">
+      <c r="G27" s="2">
         <v>64.8</v>
       </c>
-      <c r="F27" s="2">
+      <c r="H27" s="2">
         <v>56.7</v>
       </c>
-      <c r="G27" s="2">
+      <c r="I27" s="2">
         <v>32.4</v>
       </c>
-      <c r="H27" s="2">
+      <c r="J27" s="2">
         <v>35.1</v>
       </c>
-      <c r="I27" s="3">
+      <c r="K27" s="3">
         <v>29.7</v>
       </c>
-      <c r="J27" s="3">
+      <c r="L27" s="3">
         <v>40.5</v>
       </c>
-      <c r="K27" s="3">
+      <c r="M27" s="3">
         <v>62.1</v>
       </c>
-      <c r="L27" s="3">
+      <c r="N27" s="3">
         <v>64.8</v>
       </c>
-      <c r="M27" s="2">
-        <v>1</v>
-      </c>
-      <c r="N27" s="2">
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2">
         <v>2014</v>
       </c>
-      <c r="O27" s="2">
-        <v>2</v>
-      </c>
-      <c r="P27" s="2">
-        <v>2</v>
-      </c>
       <c r="Q27" s="2">
+        <v>2</v>
+      </c>
+      <c r="R27" s="2">
+        <v>2</v>
+      </c>
+      <c r="S27" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R27" t="s">
-        <v>42</v>
-      </c>
-      <c r="S27" t="s">
-        <v>43</v>
-      </c>
       <c r="T27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V27" t="s">
+        <v>43</v>
+      </c>
+      <c r="W27" t="s">
+        <v>42</v>
+      </c>
+      <c r="X27" t="s">
         <v>44</v>
       </c>
-      <c r="W27" t="s">
-        <v>42</v>
-      </c>
-      <c r="X27" t="s">
-        <v>42</v>
-      </c>
       <c r="Y27" t="s">
         <v>42</v>
       </c>
-      <c r="Z27">
+      <c r="Z27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
         <v>36</v>
       </c>
-      <c r="C28" s="2">
+      <c r="E28" s="2">
         <v>63</v>
       </c>
-      <c r="D28" s="2">
+      <c r="F28" s="2">
         <v>77</v>
       </c>
-      <c r="E28" s="2">
+      <c r="G28" s="2">
         <v>67.5</v>
       </c>
-      <c r="F28" s="2">
+      <c r="H28" s="2">
         <v>48.6</v>
       </c>
-      <c r="G28" s="2">
+      <c r="I28" s="2">
         <v>43.2</v>
       </c>
-      <c r="H28" s="2">
+      <c r="J28" s="2">
         <v>43.2</v>
       </c>
-      <c r="I28" s="4">
+      <c r="K28" s="4">
         <v>32.4</v>
       </c>
-      <c r="J28" s="4">
+      <c r="L28" s="4">
         <v>43.2</v>
       </c>
-      <c r="K28" s="4">
+      <c r="M28" s="4">
         <v>75.599999999999994</v>
       </c>
-      <c r="L28" s="4">
+      <c r="N28" s="4">
         <v>72.900000000000006</v>
       </c>
-      <c r="M28" s="2">
-        <v>1</v>
-      </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
         <v>2014</v>
       </c>
-      <c r="O28" s="2">
-        <v>2</v>
-      </c>
-      <c r="P28" s="2">
-        <v>2</v>
-      </c>
       <c r="Q28" s="2">
+        <v>2</v>
+      </c>
+      <c r="R28" s="2">
+        <v>2</v>
+      </c>
+      <c r="S28" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R28" t="s">
-        <v>42</v>
-      </c>
-      <c r="S28" t="s">
-        <v>43</v>
-      </c>
       <c r="T28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V28" t="s">
+        <v>43</v>
+      </c>
+      <c r="W28" t="s">
+        <v>42</v>
+      </c>
+      <c r="X28" t="s">
         <v>44</v>
       </c>
-      <c r="W28" t="s">
-        <v>42</v>
-      </c>
-      <c r="X28" t="s">
-        <v>42</v>
-      </c>
       <c r="Y28" t="s">
         <v>42</v>
       </c>
-      <c r="Z28">
+      <c r="Z28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB28">
         <v>7</v>
       </c>
     </row>

</xml_diff>